<commit_message>
some structures are created
</commit_message>
<xml_diff>
--- a/Instruments/trades.xlsx
+++ b/Instruments/trades.xlsx
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>Instrument</t>
-  </si>
-  <si>
     <t>2010-10-06</t>
   </si>
   <si>
@@ -54,6 +51,18 @@
   </si>
   <si>
     <t>Amount</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>HUF</t>
+  </si>
+  <si>
+    <t>Ticker</t>
   </si>
 </sst>
 </file>
@@ -371,10 +380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -382,26 +391,32 @@
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>5430</v>
@@ -409,13 +424,19 @@
       <c r="D2">
         <v>50</v>
       </c>
+      <c r="E2">
+        <v>250</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>5231</v>
@@ -423,13 +444,19 @@
       <c r="D3">
         <v>-30</v>
       </c>
+      <c r="E3">
+        <v>300</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>2438.75</v>
@@ -437,19 +464,31 @@
       <c r="D4">
         <v>23</v>
       </c>
+      <c r="E4">
+        <v>500</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>2053.75</v>
       </c>
       <c r="D5">
         <v>-12</v>
+      </c>
+      <c r="E5">
+        <v>750</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trying to write positions
</commit_message>
<xml_diff>
--- a/Instruments/trades.xlsx
+++ b/Instruments/trades.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>Ticker</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>m</t>
   </si>
 </sst>
 </file>
@@ -380,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -391,7 +397,7 @@
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -410,8 +416,11 @@
       <c r="F1" t="s">
         <v>10</v>
       </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -430,8 +439,11 @@
       <c r="F2" t="s">
         <v>11</v>
       </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -450,8 +462,11 @@
       <c r="F3" t="s">
         <v>11</v>
       </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -470,8 +485,11 @@
       <c r="F4" t="s">
         <v>11</v>
       </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -489,6 +507,9 @@
       </c>
       <c r="F5" t="s">
         <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>